<commit_message>
Inclusão do codigo de atualização da V5 na classe principal
</commit_message>
<xml_diff>
--- a/placas_veiculos.xlsx
+++ b/placas_veiculos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo Viana\Documents\Python\Bob\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005D9EAE-1CA3-4C41-8911-115402315D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA1A12-9997-4CE3-8596-94AD08EFB8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4755" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="222">
   <si>
     <t>EH056</t>
   </si>
@@ -657,6 +657,51 @@
   </si>
   <si>
     <t>IZN1I79</t>
+  </si>
+  <si>
+    <t>IYL3078</t>
+  </si>
+  <si>
+    <t>IXL3808</t>
+  </si>
+  <si>
+    <t>IXK8962</t>
+  </si>
+  <si>
+    <t>NZU5333</t>
+  </si>
+  <si>
+    <t>IZY0C31</t>
+  </si>
+  <si>
+    <t>IXW3298</t>
+  </si>
+  <si>
+    <t>ITV7358</t>
+  </si>
+  <si>
+    <t>JCY1B36</t>
+  </si>
+  <si>
+    <t>JBQ8G48</t>
+  </si>
+  <si>
+    <t>JBQ8G47</t>
+  </si>
+  <si>
+    <t>IXL3809</t>
+  </si>
+  <si>
+    <t>ITR5319</t>
+  </si>
+  <si>
+    <t>IXK8952</t>
+  </si>
+  <si>
+    <t>JBQ8G49</t>
+  </si>
+  <si>
+    <t>JBR4C61</t>
   </si>
 </sst>
 </file>
@@ -702,7 +747,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1039,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S108"/>
+  <dimension ref="A1:S123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,23 +2619,146 @@
         <v>507491</v>
       </c>
     </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>207</v>
+      </c>
+      <c r="D109">
+        <v>495692</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>208</v>
+      </c>
+      <c r="D110">
+        <v>227373</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>209</v>
+      </c>
+      <c r="D111">
+        <v>353598</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>210</v>
+      </c>
+      <c r="D112">
+        <v>515104</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>211</v>
+      </c>
+      <c r="D113">
+        <v>519556</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>212</v>
+      </c>
+      <c r="D114">
+        <v>357306</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>213</v>
+      </c>
+      <c r="D115">
+        <v>506509</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>214</v>
+      </c>
+      <c r="D116">
+        <v>563739</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>215</v>
+      </c>
+      <c r="D117">
+        <v>563727</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>216</v>
+      </c>
+      <c r="D118">
+        <v>563608</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>217</v>
+      </c>
+      <c r="D119">
+        <v>227372</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>218</v>
+      </c>
+      <c r="D120">
+        <v>327643</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>219</v>
+      </c>
+      <c r="D121">
+        <v>353579</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>220</v>
+      </c>
+      <c r="D122">
+        <v>563614</v>
+      </c>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>221</v>
+      </c>
+      <c r="D123">
+        <v>564335</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C64:C1048576 C59 C1:C53 C55">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64:C1048576 C59 C1:C55">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="C116:C117 C119:C1048576 C64:C114 C1:C59">
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64:C1048576 C1:C59">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="C116:C117 C119:C1048576 C64:C114 C59 C1:C53 C55">
+    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C116:C117 C119:C1048576 C64:C114 C59 C1:C55">
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P85:P97">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>